<commit_message>
Corrected data input errors, noted, and added columns for rounded diameter values
</commit_message>
<xml_diff>
--- a/ReadData/2020pumpkinData.xlsx
+++ b/ReadData/2020pumpkinData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suggb\Documents\ST542\Project\PumpkinProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suggb\Documents\ST542\Project\PumpkinProject\ReadData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C5E317-4D69-401A-AA05-C5801E28362B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D0AE76-A95C-40DC-9C53-FA5611414A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="-3336" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spacing Weight" sheetId="1" r:id="rId1"/>
@@ -6850,8 +6850,8 @@
       <c r="O18">
         <v>13</v>
       </c>
-      <c r="P18">
-        <v>17</v>
+      <c r="P18" s="10">
+        <v>14</v>
       </c>
       <c r="Q18">
         <v>12.8</v>

</xml_diff>